<commit_message>
feat: Extended OpenRowSet illustration to include writing as well as reading
</commit_message>
<xml_diff>
--- a/Sql/OpenRowSet/My-Shopping-List.xlsx
+++ b/Sql/OpenRowSet/My-Shopping-List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SheetRead" sheetId="1" r:id="rId1"/>
+    <sheet name="SheetWrite" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -90,6 +90,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -137,7 +140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,7 +175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,7 +387,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,12 +454,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>